<commit_message>
updated readabilty index excel with graph
</commit_message>
<xml_diff>
--- a/Readability/readability_results_sorted.xlsx
+++ b/Readability/readability_results_sorted.xlsx
@@ -2,28 +2,30 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UC Irvine\01 - Academics\3_Spring 24\EECS232 Data Privacy\Project\data_privacy_readability_ws\Readability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74007563-F3C5-4103-B2EE-AD0E629165A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E7BD63-69A6-4DD0-92E6-E550DE9E4DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20355" yWindow="2925" windowWidth="17895" windowHeight="14700" xr2:uid="{9FE58981-A030-48B7-BDE4-47B605489D3A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{9FE58981-A030-48B7-BDE4-47B605489D3A}"/>
   </bookViews>
   <sheets>
     <sheet name="readability_results" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">readability_results!$A$1:$L$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$E$18</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="51">
   <si>
     <t>Meta</t>
   </si>
@@ -165,11 +167,26 @@
   <si>
     <t>sentence info:s'</t>
   </si>
+  <si>
+    <t>Meta EU</t>
+  </si>
+  <si>
+    <t>Meta US</t>
+  </si>
+  <si>
+    <t>WhatsApp EU</t>
+  </si>
+  <si>
+    <t>WhatsApp US</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -662,12 +679,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -724,6 +744,1441 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Readability Index Trends - Whatsapp and Meta</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.4892476987883723E-2"/>
+          <c:y val="0.15902762405905005"/>
+          <c:w val="0.87532968945681044"/>
+          <c:h val="0.64400671474018956"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>WhatsApp EU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="76200" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$A$2:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>[$-409]mmmm\ d\,\ yyyy;@</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>45338</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45287</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45264</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45124</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45092</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44927</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44879</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44768</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44630</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44522</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44200</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44032</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43818</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43214</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42622</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>42607</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>41097</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$2:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>17.095412634649101</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.095412634649101</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.095412634649101</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.971515144875099</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.6794562772189</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16.6794562772189</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16.6794562772189</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16.8004243738533</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16.8004243738533</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17.034600183851101</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15.5819710276189</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16.028324756101402</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16.028324756101402</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>16.028324756101402</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13.0793438881757</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>13.0793438881757</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>19.6280318543307</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FBFA-4212-8A5F-0A1A7EB67112}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>WhatsApp US</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="76200" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:prstDash val="lgDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$2:$C$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>14.3932570617302</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.3932570617302</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.3932570617302</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.3932570617302</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.3932570617302</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14.3932570617302</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14.3932570617302</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14.3932570617302</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14.3932570617302</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.3932570617302</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14.3932570617302</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13.267063432835799</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.1443690153455</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.0793438881757</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13.0793438881757</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>13.0793438881757</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>19.6280318543307</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FBFA-4212-8A5F-0A1A7EB67112}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Meta EU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="76200" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$D$2:$D$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>18.7466172726016</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18.7466172726016</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18.707954663803001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18.707954663803001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.707954663803001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17.893871099854501</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19.881484747603501</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19.881484747603501</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.452621124334399</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15.452621124334399</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15.452621124334399</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13.4084611308639</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.4084611308639</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.4084611308639</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13.4084611308639</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-FBFA-4212-8A5F-0A1A7EB67112}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Meta US</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="57150" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="002060"/>
+              </a:solidFill>
+              <a:prstDash val="dashDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$E$2:$E$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>18.8895049008269</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18.8895049008269</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18.854853597680101</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18.854853597680101</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.854853597680101</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18.159799326796801</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19.881484747603501</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19.881484747603501</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.452621124334399</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15.452621124334399</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15.452621124334399</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13.4084611308639</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.4084611308639</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.4084611308639</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13.4084611308639</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-FBFA-4212-8A5F-0A1A7EB67112}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="608625008"/>
+        <c:axId val="608610608"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="608625008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="45658"/>
+          <c:min val="40909"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="75000"/>
+                  <a:alpha val="33000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mj-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Dates</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mj-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="[$-409]mmm/yy;@" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="608610608"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+        <c:majorUnit val="1"/>
+        <c:majorTimeUnit val="years"/>
+        <c:minorUnit val="6"/>
+        <c:minorTimeUnit val="months"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="608610608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="10"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="90000"/>
+                  <a:alpha val="24000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mj-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>ARI readability Index</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mj-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="608625008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr anchor="ctr" anchorCtr="0"/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="2000">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:latin typeface="+mj-lt"/>
+          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>538369</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>52180</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>115955</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>107674</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9FC82E9B-AEDF-B748-378C-0BFE23395E43}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1043,17 +2498,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE773D15-C3A2-4B50-9ADC-8BCA9C5A31DC}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:BQ32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
@@ -1076,10 +2530,10 @@
         <v>7</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>12</v>
@@ -1112,7 +2566,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:69" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1123,10 +2577,10 @@
         <v>6</v>
       </c>
       <c r="D2" s="2">
+        <v>15.6745905262897</v>
+      </c>
+      <c r="E2" s="2">
         <v>13.8603450025931</v>
-      </c>
-      <c r="E2" s="2">
-        <v>15.6745905262897</v>
       </c>
       <c r="F2" s="2">
         <v>13.7346899664369</v>
@@ -1318,7 +2772,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:69" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1329,10 +2783,10 @@
         <v>6</v>
       </c>
       <c r="D3" s="2">
+        <v>11.8765889666821</v>
+      </c>
+      <c r="E3" s="2">
         <v>10.7621662120139</v>
-      </c>
-      <c r="E3" s="2">
-        <v>11.8765889666821</v>
       </c>
       <c r="F3" s="2">
         <v>11.332021062821701</v>
@@ -1524,7 +2978,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:69" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1535,10 +2989,10 @@
         <v>5</v>
       </c>
       <c r="D4" s="2">
+        <v>17.095412634649101</v>
+      </c>
+      <c r="E4" s="2">
         <v>14.8580413378647</v>
-      </c>
-      <c r="E4" s="2">
-        <v>17.095412634649101</v>
       </c>
       <c r="F4" s="2">
         <v>13.8790491277031</v>
@@ -1730,7 +3184,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:69" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -1741,10 +3195,10 @@
         <v>5</v>
       </c>
       <c r="D5" s="2">
+        <v>11.915977005498601</v>
+      </c>
+      <c r="E5" s="2">
         <v>10.544093417274601</v>
-      </c>
-      <c r="E5" s="2">
-        <v>11.915977005498601</v>
       </c>
       <c r="F5" s="2">
         <v>11.2358361439153</v>
@@ -1947,10 +3401,10 @@
         <v>5</v>
       </c>
       <c r="D6" s="2">
+        <v>18.7466172726016</v>
+      </c>
+      <c r="E6" s="2">
         <v>16.057866212720899</v>
-      </c>
-      <c r="E6" s="2">
-        <v>18.7466172726016</v>
       </c>
       <c r="F6" s="2">
         <v>13.032940023003301</v>
@@ -2153,10 +3607,10 @@
         <v>6</v>
       </c>
       <c r="D7" s="2">
+        <v>18.8895049008269</v>
+      </c>
+      <c r="E7" s="2">
         <v>16.2025613557376</v>
-      </c>
-      <c r="E7" s="2">
-        <v>18.8895049008269</v>
       </c>
       <c r="F7" s="2">
         <v>13.1846824421714</v>
@@ -2348,7 +3802,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:69" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -2359,10 +3813,10 @@
         <v>5</v>
       </c>
       <c r="D8" s="2">
+        <v>17.095412634649101</v>
+      </c>
+      <c r="E8" s="2">
         <v>14.8580413378647</v>
-      </c>
-      <c r="E8" s="2">
-        <v>17.095412634649101</v>
       </c>
       <c r="F8" s="2">
         <v>13.8790491277031</v>
@@ -2554,7 +4008,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:69" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
@@ -2565,10 +4019,10 @@
         <v>5</v>
       </c>
       <c r="D9" s="2">
+        <v>14.700080285431399</v>
+      </c>
+      <c r="E9" s="2">
         <v>13.0858792815764</v>
-      </c>
-      <c r="E9" s="2">
-        <v>14.700080285431399</v>
       </c>
       <c r="F9" s="2">
         <v>14.304046346314299</v>
@@ -2771,10 +4225,10 @@
         <v>5</v>
       </c>
       <c r="D10" s="2">
+        <v>18.707954663803001</v>
+      </c>
+      <c r="E10" s="2">
         <v>16.028972572819601</v>
-      </c>
-      <c r="E10" s="2">
-        <v>18.707954663803001</v>
       </c>
       <c r="F10" s="2">
         <v>13.022219048461</v>
@@ -2977,10 +4431,10 @@
         <v>6</v>
       </c>
       <c r="D11" s="2">
+        <v>18.854853597680101</v>
+      </c>
+      <c r="E11" s="2">
         <v>16.1766729177771</v>
-      </c>
-      <c r="E11" s="2">
-        <v>18.854853597680101</v>
       </c>
       <c r="F11" s="2">
         <v>13.1751266812892</v>
@@ -3172,7 +4626,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:69" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
@@ -3183,10 +4637,10 @@
         <v>5</v>
       </c>
       <c r="D12" s="2">
+        <v>16.971515144875099</v>
+      </c>
+      <c r="E12" s="2">
         <v>14.7264768353163</v>
-      </c>
-      <c r="E12" s="2">
-        <v>16.971515144875099</v>
       </c>
       <c r="F12" s="2">
         <v>13.870680920013699</v>
@@ -3389,10 +4843,10 @@
         <v>5</v>
       </c>
       <c r="D13" s="2">
+        <v>17.893871099854501</v>
+      </c>
+      <c r="E13" s="2">
         <v>15.331419410464999</v>
-      </c>
-      <c r="E13" s="2">
-        <v>17.893871099854501</v>
       </c>
       <c r="F13" s="2">
         <v>12.808579608535799</v>
@@ -3595,10 +5049,10 @@
         <v>6</v>
       </c>
       <c r="D14" s="2">
+        <v>18.159799326796801</v>
+      </c>
+      <c r="E14" s="2">
         <v>15.585148307653901</v>
-      </c>
-      <c r="E14" s="2">
-        <v>18.159799326796801</v>
       </c>
       <c r="F14" s="2">
         <v>13.013155622379401</v>
@@ -3801,10 +5255,10 @@
         <v>5</v>
       </c>
       <c r="D15" s="2">
+        <v>19.881484747603501</v>
+      </c>
+      <c r="E15" s="2">
         <v>17.260049050856999</v>
-      </c>
-      <c r="E15" s="2">
-        <v>19.881484747603501</v>
       </c>
       <c r="F15" s="2">
         <v>14.467303549936201</v>
@@ -4007,10 +5461,10 @@
         <v>6</v>
       </c>
       <c r="D16" s="2">
+        <v>19.881484747603501</v>
+      </c>
+      <c r="E16" s="2">
         <v>17.260049050856999</v>
-      </c>
-      <c r="E16" s="2">
-        <v>19.881484747603501</v>
       </c>
       <c r="F16" s="2">
         <v>14.467303549936201</v>
@@ -4202,7 +5656,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:69" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>4</v>
       </c>
@@ -4213,10 +5667,10 @@
         <v>5</v>
       </c>
       <c r="D17" s="2">
+        <v>16.6794562772189</v>
+      </c>
+      <c r="E17" s="2">
         <v>14.472168281527701</v>
-      </c>
-      <c r="E17" s="2">
-        <v>16.6794562772189</v>
       </c>
       <c r="F17" s="2">
         <v>13.8555743561715</v>
@@ -4408,7 +5862,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:69" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>4</v>
       </c>
@@ -4419,10 +5873,10 @@
         <v>5</v>
       </c>
       <c r="D18" s="2">
+        <v>16.8004243738533</v>
+      </c>
+      <c r="E18" s="2">
         <v>14.508187429704</v>
-      </c>
-      <c r="E18" s="2">
-        <v>16.8004243738533</v>
       </c>
       <c r="F18" s="2">
         <v>13.7925516750922</v>
@@ -4625,10 +6079,10 @@
         <v>5</v>
       </c>
       <c r="D19" s="2">
+        <v>15.452621124334399</v>
+      </c>
+      <c r="E19" s="2">
         <v>13.570529282806101</v>
-      </c>
-      <c r="E19" s="2">
-        <v>15.452621124334399</v>
       </c>
       <c r="F19" s="2">
         <v>12.5381417978155</v>
@@ -4831,10 +6285,10 @@
         <v>6</v>
       </c>
       <c r="D20" s="2">
+        <v>15.452621124334399</v>
+      </c>
+      <c r="E20" s="2">
         <v>13.570529282806101</v>
-      </c>
-      <c r="E20" s="2">
-        <v>15.452621124334399</v>
       </c>
       <c r="F20" s="2">
         <v>12.5381417978155</v>
@@ -5026,7 +6480,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:69" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>4</v>
       </c>
@@ -5037,10 +6491,10 @@
         <v>5</v>
       </c>
       <c r="D21" s="2">
+        <v>17.034600183851101</v>
+      </c>
+      <c r="E21" s="2">
         <v>14.7198088410991</v>
-      </c>
-      <c r="E21" s="2">
-        <v>17.034600183851101</v>
       </c>
       <c r="F21" s="2">
         <v>13.876921569096901</v>
@@ -5232,7 +6686,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:69" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>4</v>
       </c>
@@ -5243,10 +6697,10 @@
         <v>5</v>
       </c>
       <c r="D22" s="2">
+        <v>15.5819710276189</v>
+      </c>
+      <c r="E22" s="2">
         <v>13.9803380569067</v>
-      </c>
-      <c r="E22" s="2">
-        <v>15.5819710276189</v>
       </c>
       <c r="F22" s="2">
         <v>13.5767093748397</v>
@@ -5438,7 +6892,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:69" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>4</v>
       </c>
@@ -5449,10 +6903,10 @@
         <v>6</v>
       </c>
       <c r="D23" s="2">
+        <v>14.3932570617302</v>
+      </c>
+      <c r="E23" s="2">
         <v>12.9082454458293</v>
-      </c>
-      <c r="E23" s="2">
-        <v>14.3932570617302</v>
       </c>
       <c r="F23" s="2">
         <v>13.3210607576701</v>
@@ -5644,7 +7098,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:69" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>4</v>
       </c>
@@ -5655,10 +7109,10 @@
         <v>6</v>
       </c>
       <c r="D24" s="2">
+        <v>13.267063432835799</v>
+      </c>
+      <c r="E24" s="2">
         <v>11.955405970149201</v>
-      </c>
-      <c r="E24" s="2">
-        <v>13.267063432835799</v>
       </c>
       <c r="F24" s="2">
         <v>12.7515830123134</v>
@@ -5850,7 +7304,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:69" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>4</v>
       </c>
@@ -5861,10 +7315,10 @@
         <v>6</v>
       </c>
       <c r="D25" s="2">
+        <v>13.1443690153455</v>
+      </c>
+      <c r="E25" s="2">
         <v>11.8515861665879</v>
-      </c>
-      <c r="E25" s="2">
-        <v>13.1443690153455</v>
       </c>
       <c r="F25" s="2">
         <v>12.8890488955281</v>
@@ -6056,7 +7510,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:69" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>4</v>
       </c>
@@ -6067,10 +7521,10 @@
         <v>5</v>
       </c>
       <c r="D26" s="2">
+        <v>16.028324756101402</v>
+      </c>
+      <c r="E26" s="2">
         <v>14.2333389006409</v>
-      </c>
-      <c r="E26" s="2">
-        <v>16.028324756101402</v>
       </c>
       <c r="F26" s="2">
         <v>13.4078928104379</v>
@@ -6273,10 +7727,10 @@
         <v>5</v>
       </c>
       <c r="D27" s="2">
+        <v>13.4084611308639</v>
+      </c>
+      <c r="E27" s="2">
         <v>12.2398801662998</v>
-      </c>
-      <c r="E27" s="2">
-        <v>13.4084611308639</v>
       </c>
       <c r="F27" s="2">
         <v>11.877761117754901</v>
@@ -6479,10 +7933,10 @@
         <v>6</v>
       </c>
       <c r="D28" s="2">
+        <v>13.4084611308639</v>
+      </c>
+      <c r="E28" s="2">
         <v>12.2398801662998</v>
-      </c>
-      <c r="E28" s="2">
-        <v>13.4084611308639</v>
       </c>
       <c r="F28" s="2">
         <v>11.877761117754901</v>
@@ -6674,7 +8128,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:69" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>4</v>
       </c>
@@ -6685,10 +8139,10 @@
         <v>5</v>
       </c>
       <c r="D29" s="2">
+        <v>13.0793438881757</v>
+      </c>
+      <c r="E29" s="2">
         <v>11.7909580183521</v>
-      </c>
-      <c r="E29" s="2">
-        <v>13.0793438881757</v>
       </c>
       <c r="F29" s="2">
         <v>12.8444242358674</v>
@@ -6880,7 +8334,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:69" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>4</v>
       </c>
@@ -6891,10 +8345,10 @@
         <v>6</v>
       </c>
       <c r="D30" s="2">
+        <v>13.0793438881757</v>
+      </c>
+      <c r="E30" s="2">
         <v>11.7909580183521</v>
-      </c>
-      <c r="E30" s="2">
-        <v>13.0793438881757</v>
       </c>
       <c r="F30" s="2">
         <v>12.8444242358674</v>
@@ -7086,7 +8540,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:69" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>4</v>
       </c>
@@ -7097,10 +8551,10 @@
         <v>5</v>
       </c>
       <c r="D31" s="2">
+        <v>19.6280318543307</v>
+      </c>
+      <c r="E31" s="2">
         <v>16.465115654858</v>
-      </c>
-      <c r="E31" s="2">
-        <v>19.6280318543307</v>
       </c>
       <c r="F31" s="2">
         <v>13.643549939633401</v>
@@ -7292,7 +8746,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:69" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>4</v>
       </c>
@@ -7303,10 +8757,10 @@
         <v>6</v>
       </c>
       <c r="D32" s="2">
+        <v>19.6280318543307</v>
+      </c>
+      <c r="E32" s="2">
         <v>16.465115654858</v>
-      </c>
-      <c r="E32" s="2">
-        <v>19.6280318543307</v>
       </c>
       <c r="F32" s="2">
         <v>13.643549939633401</v>
@@ -7500,15 +8954,338 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:L32" xr:uid="{FE773D15-C3A2-4B50-9ADC-8BCA9C5A31DC}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Meta"/>
-      </filters>
-    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:L28">
       <sortCondition descending="1" ref="B1:B32"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E238B8C-CD75-4E94-B7DA-1526F7482999}">
+  <dimension ref="A1:E18"/>
+  <sheetViews>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="Y25" sqref="Y25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>45338</v>
+      </c>
+      <c r="B2" s="2">
+        <v>17.095412634649101</v>
+      </c>
+      <c r="C2" s="2">
+        <v>14.3932570617302</v>
+      </c>
+      <c r="D2" s="2">
+        <v>18.7466172726016</v>
+      </c>
+      <c r="E2" s="2">
+        <v>18.8895049008269</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>45287</v>
+      </c>
+      <c r="B3" s="2">
+        <v>17.095412634649101</v>
+      </c>
+      <c r="C3" s="2">
+        <v>14.3932570617302</v>
+      </c>
+      <c r="D3" s="2">
+        <v>18.7466172726016</v>
+      </c>
+      <c r="E3" s="2">
+        <v>18.8895049008269</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>45264</v>
+      </c>
+      <c r="B4" s="2">
+        <v>17.095412634649101</v>
+      </c>
+      <c r="C4" s="2">
+        <v>14.3932570617302</v>
+      </c>
+      <c r="D4" s="2">
+        <v>18.707954663803001</v>
+      </c>
+      <c r="E4" s="2">
+        <v>18.854853597680101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>45124</v>
+      </c>
+      <c r="B5" s="2">
+        <v>16.971515144875099</v>
+      </c>
+      <c r="C5" s="2">
+        <v>14.3932570617302</v>
+      </c>
+      <c r="D5" s="2">
+        <v>18.707954663803001</v>
+      </c>
+      <c r="E5" s="2">
+        <v>18.854853597680101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>45092</v>
+      </c>
+      <c r="B6" s="2">
+        <v>16.6794562772189</v>
+      </c>
+      <c r="C6" s="2">
+        <v>14.3932570617302</v>
+      </c>
+      <c r="D6" s="2">
+        <v>18.707954663803001</v>
+      </c>
+      <c r="E6" s="2">
+        <v>18.854853597680101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>44927</v>
+      </c>
+      <c r="B7" s="2">
+        <v>16.6794562772189</v>
+      </c>
+      <c r="C7" s="2">
+        <v>14.3932570617302</v>
+      </c>
+      <c r="D7" s="2">
+        <v>17.893871099854501</v>
+      </c>
+      <c r="E7" s="2">
+        <v>18.159799326796801</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>44879</v>
+      </c>
+      <c r="B8" s="2">
+        <v>16.6794562772189</v>
+      </c>
+      <c r="C8" s="2">
+        <v>14.3932570617302</v>
+      </c>
+      <c r="D8" s="2">
+        <v>19.881484747603501</v>
+      </c>
+      <c r="E8" s="2">
+        <v>19.881484747603501</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>44768</v>
+      </c>
+      <c r="B9" s="2">
+        <v>16.8004243738533</v>
+      </c>
+      <c r="C9" s="2">
+        <v>14.3932570617302</v>
+      </c>
+      <c r="D9" s="2">
+        <v>19.881484747603501</v>
+      </c>
+      <c r="E9" s="2">
+        <v>19.881484747603501</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>44630</v>
+      </c>
+      <c r="B10" s="2">
+        <v>16.8004243738533</v>
+      </c>
+      <c r="C10" s="2">
+        <v>14.3932570617302</v>
+      </c>
+      <c r="D10" s="2">
+        <v>15.452621124334399</v>
+      </c>
+      <c r="E10" s="2">
+        <v>15.452621124334399</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>44522</v>
+      </c>
+      <c r="B11" s="2">
+        <v>17.034600183851101</v>
+      </c>
+      <c r="C11" s="2">
+        <v>14.3932570617302</v>
+      </c>
+      <c r="D11" s="2">
+        <v>15.452621124334399</v>
+      </c>
+      <c r="E11" s="2">
+        <v>15.452621124334399</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>44200</v>
+      </c>
+      <c r="B12" s="2">
+        <v>15.5819710276189</v>
+      </c>
+      <c r="C12" s="2">
+        <v>14.3932570617302</v>
+      </c>
+      <c r="D12" s="2">
+        <v>15.452621124334399</v>
+      </c>
+      <c r="E12" s="2">
+        <v>15.452621124334399</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>44032</v>
+      </c>
+      <c r="B13" s="2">
+        <v>16.028324756101402</v>
+      </c>
+      <c r="C13" s="2">
+        <v>13.267063432835799</v>
+      </c>
+      <c r="D13" s="2">
+        <v>13.4084611308639</v>
+      </c>
+      <c r="E13" s="2">
+        <v>13.4084611308639</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>43818</v>
+      </c>
+      <c r="B14" s="2">
+        <v>16.028324756101402</v>
+      </c>
+      <c r="C14" s="2">
+        <v>13.1443690153455</v>
+      </c>
+      <c r="D14" s="2">
+        <v>13.4084611308639</v>
+      </c>
+      <c r="E14" s="2">
+        <v>13.4084611308639</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>43214</v>
+      </c>
+      <c r="B15" s="2">
+        <v>16.028324756101402</v>
+      </c>
+      <c r="C15" s="2">
+        <v>13.0793438881757</v>
+      </c>
+      <c r="D15" s="2">
+        <v>13.4084611308639</v>
+      </c>
+      <c r="E15" s="2">
+        <v>13.4084611308639</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>42622</v>
+      </c>
+      <c r="B16" s="2">
+        <v>13.0793438881757</v>
+      </c>
+      <c r="C16" s="2">
+        <v>13.0793438881757</v>
+      </c>
+      <c r="D16" s="2">
+        <v>13.4084611308639</v>
+      </c>
+      <c r="E16" s="2">
+        <v>13.4084611308639</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>42607</v>
+      </c>
+      <c r="B17" s="2">
+        <v>13.0793438881757</v>
+      </c>
+      <c r="C17" s="2">
+        <v>13.0793438881757</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>41097</v>
+      </c>
+      <c r="B18" s="2">
+        <v>19.6280318543307</v>
+      </c>
+      <c r="C18" s="2">
+        <v>19.6280318543307</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E18" xr:uid="{5E238B8C-CD75-4E94-B7DA-1526F7482999}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E18">
+      <sortCondition descending="1" ref="A1:A18"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added gpt results for compliance
</commit_message>
<xml_diff>
--- a/Readability/readability_results_sorted.xlsx
+++ b/Readability/readability_results_sorted.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UC Irvine\01 - Academics\3_Spring 24\EECS232 Data Privacy\Project\data_privacy_readability_ws\Readability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E7BD63-69A6-4DD0-92E6-E550DE9E4DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58C36B7-A216-485D-A5C8-1305F1A457DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{9FE58981-A030-48B7-BDE4-47B605489D3A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{9FE58981-A030-48B7-BDE4-47B605489D3A}"/>
   </bookViews>
   <sheets>
     <sheet name="readability_results" sheetId="1" r:id="rId1"/>
@@ -185,7 +185,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -685,9 +685,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -852,6 +852,9 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>Sheet2!$A$2:$A$18</c:f>
@@ -1006,6 +1009,9 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>Sheet2!$C$2:$C$18</c:f>
@@ -1100,6 +1106,9 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>Sheet2!$D$2:$D$18</c:f>
@@ -1188,6 +1197,9 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>Sheet2!$E$2:$E$18</c:f>
@@ -1250,9 +1262,8 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -1439,9 +1450,10 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>ARI readability Index</a:t>
+                  <a:rPr lang="en-US" sz="2000" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+                  <a:t>Automated Readability Index (ARI)</a:t>
                 </a:r>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2145,15 +2157,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>538369</xdr:colOff>
+      <xdr:colOff>173182</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>52180</xdr:rowOff>
+      <xdr:rowOff>26203</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>115955</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>107674</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>17317</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>121227</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2500,7 +2512,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE773D15-C3A2-4B50-9ADC-8BCA9C5A31DC}">
   <dimension ref="A1:BQ32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
@@ -8966,8 +8978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E238B8C-CD75-4E94-B7DA-1526F7482999}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="Y25" sqref="Y25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="Y28" sqref="Y28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>